<commit_message>
actualisacion de proyecto y de docuemntacion
se actualizo todo el royecto web y se actualisaron algunos ducuemntos
del repositorio
</commit_message>
<xml_diff>
--- a/Administracion-de-Proyectos/Aseguramiento-de-la-calidad/TMv3-Repositorio-de-Lecciones-Aprendidas.xlsx
+++ b/Administracion-de-Proyectos/Aseguramiento-de-la-calidad/TMv3-Repositorio-de-Lecciones-Aprendidas.xlsx
@@ -281,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="257">
   <si>
     <t>PP</t>
   </si>
@@ -925,13 +925,142 @@
   </si>
   <si>
     <t>Sergio Alan Orrala Silva</t>
+  </si>
+  <si>
+    <t>REQM</t>
+  </si>
+  <si>
+    <t>Codificación</t>
+  </si>
+  <si>
+    <t>Agregar comentarios sobre el codiogo del sitio web</t>
+  </si>
+  <si>
+    <t>Documentación inadecuada sobre el código del sitio web</t>
+  </si>
+  <si>
+    <t>Agregar comentarios sobre el titulo de los distintos apartados de la sitio web en el código</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Plan de CM</t>
+  </si>
+  <si>
+    <t>Definición correcta de la configuración de los archivos administrativos del proyecto</t>
+  </si>
+  <si>
+    <t>Desconocimiento de la definición de configuración de los archivos administrativos del proyecto</t>
+  </si>
+  <si>
+    <t>Publicar y dar a conocer la definición de configuración de los archivos administrativos del proyecto</t>
+  </si>
+  <si>
+    <t>Correcta y adecuada definición del proceso de control de cambios de los documentos del desarrollo del proyecto</t>
+  </si>
+  <si>
+    <t>Mala definición del proceso de control de cambios de los documentos del desarrollo del proyecto</t>
+  </si>
+  <si>
+    <t>Definir clara y sencillamente cada uno de los pasos del proceso de control de cambios de los documentos del desarrollo del proyecto</t>
+  </si>
+  <si>
+    <t>Diagrama de Gantt (WBS)</t>
+  </si>
+  <si>
+    <t>Fases de desarrollo del proyecto de acuerdo al ciclo de vida seleccionado</t>
+  </si>
+  <si>
+    <t>Omitir fases de desarrollo del proyecto de acuerdo al ciclo de vida seleccionado</t>
+  </si>
+  <si>
+    <t>Desarrollar fases de desarrollo del proyecto de acuerdo al ciclo de vida seleccionado</t>
+  </si>
+  <si>
+    <t>Planeación</t>
+  </si>
+  <si>
+    <t>Desarrollo de una adecuada planeación para el desarrollo del proyecto</t>
+  </si>
+  <si>
+    <t>No realizar una adecuada planeación para el desarrollo del proyecto</t>
+  </si>
+  <si>
+    <t>Realizar una planeación realista que permita cumplir con los tiempos, costos y alcances del proyecto</t>
+  </si>
+  <si>
+    <t>Plan de Alcance</t>
+  </si>
+  <si>
+    <t>Correcta definición de los criterios de aceptación de cada alcance del proyecto</t>
+  </si>
+  <si>
+    <t>Mala definición de criterios de aceptación de cada uno de los alcances del proyecto</t>
+  </si>
+  <si>
+    <t>Realizar una descripción clara y conscisa de cada criterio de aceptación de los alcances del proyecto</t>
+  </si>
+  <si>
+    <t>Especificación de requerimientos funcionales y no funcionales</t>
+  </si>
+  <si>
+    <t>Correcta definición de requerimientos funcionales y no funcionales</t>
+  </si>
+  <si>
+    <t>Inadecuada definición de requerimientos funcionales y no funcionales</t>
+  </si>
+  <si>
+    <t>Definir cada uno de los requerimientos funcionales y no funcionales de forma concreta, clara y consisa</t>
+  </si>
+  <si>
+    <t>Definicion de estrategia de recoleccion de requerimientos</t>
+  </si>
+  <si>
+    <t>Buena elección de estrategia de recolección de requerimientos</t>
+  </si>
+  <si>
+    <t>Mala elección de estrategia de recolección de requerimientos</t>
+  </si>
+  <si>
+    <t>Seleccionar una estrategia de recolección de requerimientos que se adecue a la situación real de la empresa, de los process y de los usuarios finales</t>
+  </si>
+  <si>
+    <t>Correcta priorización y jerarquización de los requerimientos funcionales y no funcionales</t>
+  </si>
+  <si>
+    <t>Priorización y jerarquización inadecuada de los requerimientos funcionales y no funcionales</t>
+  </si>
+  <si>
+    <t>Priorizar y jerarquizar los requerimientos funcionales y no funcionales bajo un criterio basado en los alcances del proyecto</t>
+  </si>
+  <si>
+    <t>Correcta decripción y capacitación de uso de la herramienta de Gestión de Configuración</t>
+  </si>
+  <si>
+    <t>Descripción y capacitación de uso incompleta de la herramienta de Gestión de Configuración</t>
+  </si>
+  <si>
+    <t>Describir la herramienta de Gestión de Configuración y desarrollar un manual breve y consiso de su uso y sus principales funciones</t>
+  </si>
+  <si>
+    <t>Minuta</t>
+  </si>
+  <si>
+    <t>Seguir manteniendo la linea base</t>
+  </si>
+  <si>
+    <t>Buena definición de la linea base</t>
+  </si>
+  <si>
+    <t>Mejorar la linea base [noombre]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -995,6 +1124,10 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1200,10 +1333,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1311,6 +1445,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1341,36 +1502,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1734,21 +1884,21 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:4" s="2" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41"/>
+      <c r="C3" s="50"/>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:4" s="2" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="42"/>
+      <c r="B5" s="51"/>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -1818,10 +1968,10 @@
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="38"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
     </row>
@@ -1864,10 +2014,10 @@
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
@@ -1910,12 +2060,12 @@
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="38"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="47"/>
     </row>
     <row r="27" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
@@ -2097,8 +2247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,41 +2268,41 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
       <c r="M2" s="33"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
       <c r="F3" s="34"/>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
       <c r="J3" s="34"/>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="L3" s="45"/>
+      <c r="L3" s="54"/>
     </row>
     <row r="4" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
@@ -2189,7 +2339,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="37" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="32" t="s">
@@ -2224,7 +2374,7 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="37" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="32" t="s">
@@ -2259,7 +2409,7 @@
       <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:13" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="37" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="32" t="s">
@@ -2294,7 +2444,7 @@
       <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:13" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="37" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="32" t="s">
@@ -2329,7 +2479,7 @@
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="37" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="32" t="s">
@@ -2364,7 +2514,7 @@
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="37" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="32" t="s">
@@ -2399,7 +2549,7 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="37" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="32" t="s">
@@ -2434,7 +2584,7 @@
       <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:13" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="37" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="32" t="s">
@@ -2469,7 +2619,7 @@
       <c r="M12" s="7"/>
     </row>
     <row r="13" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="37" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="32" t="s">
@@ -2504,7 +2654,7 @@
       <c r="M13" s="7"/>
     </row>
     <row r="14" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="37" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="32" t="s">
@@ -2539,7 +2689,7 @@
       <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="38" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="32" t="s">
@@ -2555,7 +2705,7 @@
         <v>104</v>
       </c>
       <c r="F15" s="32"/>
-      <c r="G15" s="52" t="s">
+      <c r="G15" s="42" t="s">
         <v>105</v>
       </c>
       <c r="H15" s="32" t="s">
@@ -2574,7 +2724,7 @@
       <c r="M15" s="7"/>
     </row>
     <row r="16" spans="1:13" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="38" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="32" t="s">
@@ -2590,13 +2740,13 @@
         <v>108</v>
       </c>
       <c r="F16" s="32"/>
-      <c r="G16" s="53" t="s">
+      <c r="G16" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="H16" s="54" t="s">
+      <c r="H16" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="I16" s="54" t="s">
+      <c r="I16" s="44" t="s">
         <v>111</v>
       </c>
       <c r="J16" s="8"/>
@@ -2609,7 +2759,7 @@
       <c r="M16" s="6"/>
     </row>
     <row r="17" spans="1:13" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="38" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="32" t="s">
@@ -2625,13 +2775,13 @@
         <v>112</v>
       </c>
       <c r="F17" s="32"/>
-      <c r="G17" s="53" t="s">
+      <c r="G17" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="H17" s="53" t="s">
+      <c r="H17" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="I17" s="54" t="s">
+      <c r="I17" s="44" t="s">
         <v>115</v>
       </c>
       <c r="J17" s="8"/>
@@ -2644,7 +2794,7 @@
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="38" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="32" t="s">
@@ -2660,13 +2810,13 @@
         <v>116</v>
       </c>
       <c r="F18" s="32"/>
-      <c r="G18" s="53" t="s">
+      <c r="G18" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="H18" s="55" t="s">
+      <c r="H18" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="I18" s="53" t="s">
+      <c r="I18" s="43" t="s">
         <v>119</v>
       </c>
       <c r="J18" s="8"/>
@@ -2679,7 +2829,7 @@
       <c r="M18" s="6"/>
     </row>
     <row r="19" spans="1:13" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="38" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="32" t="s">
@@ -2695,13 +2845,13 @@
         <v>120</v>
       </c>
       <c r="F19" s="32"/>
-      <c r="G19" s="54" t="s">
+      <c r="G19" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="H19" s="54" t="s">
+      <c r="H19" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="I19" s="54" t="s">
+      <c r="I19" s="44" t="s">
         <v>123</v>
       </c>
       <c r="J19" s="8"/>
@@ -2714,7 +2864,7 @@
       <c r="M19" s="6"/>
     </row>
     <row r="20" spans="1:13" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="38" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="32" t="s">
@@ -2730,13 +2880,13 @@
         <v>124</v>
       </c>
       <c r="F20" s="32"/>
-      <c r="G20" s="54" t="s">
+      <c r="G20" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="H20" s="54" t="s">
+      <c r="H20" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="I20" s="54" t="s">
+      <c r="I20" s="44" t="s">
         <v>127</v>
       </c>
       <c r="J20" s="8"/>
@@ -2749,7 +2899,7 @@
       <c r="M20" s="6"/>
     </row>
     <row r="21" spans="1:13" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="38" t="s">
         <v>44</v>
       </c>
       <c r="B21" s="32" t="s">
@@ -2765,13 +2915,13 @@
         <v>128</v>
       </c>
       <c r="F21" s="32"/>
-      <c r="G21" s="53" t="s">
+      <c r="G21" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="H21" s="54" t="s">
+      <c r="H21" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="I21" s="54" t="s">
+      <c r="I21" s="44" t="s">
         <v>131</v>
       </c>
       <c r="J21" s="8"/>
@@ -2784,7 +2934,7 @@
       <c r="M21" s="6"/>
     </row>
     <row r="22" spans="1:13" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="38" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="32" t="s">
@@ -2800,13 +2950,13 @@
         <v>132</v>
       </c>
       <c r="F22" s="32"/>
-      <c r="G22" s="54" t="s">
+      <c r="G22" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="H22" s="54" t="s">
+      <c r="H22" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="I22" s="54" t="s">
+      <c r="I22" s="44" t="s">
         <v>135</v>
       </c>
       <c r="J22" s="8"/>
@@ -2819,7 +2969,7 @@
       <c r="M22" s="6"/>
     </row>
     <row r="23" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="38" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="32" t="s">
@@ -2835,13 +2985,13 @@
         <v>136</v>
       </c>
       <c r="F23" s="32"/>
-      <c r="G23" s="54" t="s">
+      <c r="G23" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="H23" s="54" t="s">
+      <c r="H23" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="I23" s="54" t="s">
+      <c r="I23" s="44" t="s">
         <v>139</v>
       </c>
       <c r="J23" s="8"/>
@@ -2853,8 +3003,8 @@
       </c>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="48" t="s">
+    <row r="24" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="38" t="s">
         <v>47</v>
       </c>
       <c r="B24" s="32" t="s">
@@ -2863,21 +3013,33 @@
       <c r="C24" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="6"/>
+      <c r="D24" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="F24" s="58"/>
+      <c r="G24" s="56" t="s">
+        <v>254</v>
+      </c>
+      <c r="H24" s="56" t="s">
+        <v>255</v>
+      </c>
+      <c r="I24" s="56" t="s">
+        <v>256</v>
+      </c>
+      <c r="J24" s="58"/>
+      <c r="K24" s="32" t="s">
+        <v>212</v>
+      </c>
       <c r="L24" s="32" t="s">
         <v>213</v>
       </c>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
+    <row r="25" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="32" t="s">
@@ -2886,21 +3048,33 @@
       <c r="C25" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="6"/>
+      <c r="D25" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="E25" s="57" t="s">
+        <v>215</v>
+      </c>
+      <c r="F25" s="58"/>
+      <c r="G25" s="59" t="s">
+        <v>216</v>
+      </c>
+      <c r="H25" s="59" t="s">
+        <v>217</v>
+      </c>
+      <c r="I25" s="59" t="s">
+        <v>218</v>
+      </c>
+      <c r="J25" s="58"/>
+      <c r="K25" s="32" t="s">
+        <v>212</v>
+      </c>
       <c r="L25" s="32" t="s">
         <v>213</v>
       </c>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49" t="s">
+    <row r="26" spans="1:13" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="32" t="s">
@@ -2909,21 +3083,33 @@
       <c r="C26" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="6"/>
+      <c r="D26" s="56" t="s">
+        <v>219</v>
+      </c>
+      <c r="E26" s="60" t="s">
+        <v>220</v>
+      </c>
+      <c r="F26" s="58"/>
+      <c r="G26" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="H26" s="59" t="s">
+        <v>222</v>
+      </c>
+      <c r="I26" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="J26" s="58"/>
+      <c r="K26" s="32" t="s">
+        <v>212</v>
+      </c>
       <c r="L26" s="32" t="s">
         <v>213</v>
       </c>
       <c r="M26" s="6"/>
     </row>
-    <row r="27" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="49" t="s">
+    <row r="27" spans="1:13" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="39" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="32" t="s">
@@ -2932,21 +3118,33 @@
       <c r="C27" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="6"/>
+      <c r="D27" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="60" t="s">
+        <v>220</v>
+      </c>
+      <c r="F27" s="58"/>
+      <c r="G27" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="H27" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="I27" s="59" t="s">
+        <v>226</v>
+      </c>
+      <c r="J27" s="58"/>
+      <c r="K27" s="32" t="s">
+        <v>212</v>
+      </c>
       <c r="L27" s="32" t="s">
         <v>213</v>
       </c>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="49" t="s">
+    <row r="28" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
         <v>51</v>
       </c>
       <c r="B28" s="32" t="s">
@@ -2955,21 +3153,33 @@
       <c r="C28" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="6"/>
+      <c r="D28" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="60" t="s">
+        <v>227</v>
+      </c>
+      <c r="F28" s="58"/>
+      <c r="G28" s="59" t="s">
+        <v>228</v>
+      </c>
+      <c r="H28" s="59" t="s">
+        <v>229</v>
+      </c>
+      <c r="I28" s="59" t="s">
+        <v>230</v>
+      </c>
+      <c r="J28" s="58"/>
+      <c r="K28" s="32" t="s">
+        <v>212</v>
+      </c>
       <c r="L28" s="32" t="s">
         <v>213</v>
       </c>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="s">
+    <row r="29" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
         <v>52</v>
       </c>
       <c r="B29" s="32" t="s">
@@ -2978,21 +3188,33 @@
       <c r="C29" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="6"/>
+      <c r="D29" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="60" t="s">
+        <v>231</v>
+      </c>
+      <c r="F29" s="58"/>
+      <c r="G29" s="59" t="s">
+        <v>232</v>
+      </c>
+      <c r="H29" s="59" t="s">
+        <v>233</v>
+      </c>
+      <c r="I29" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="J29" s="58"/>
+      <c r="K29" s="32" t="s">
+        <v>212</v>
+      </c>
       <c r="L29" s="32" t="s">
         <v>213</v>
       </c>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="49" t="s">
+    <row r="30" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="39" t="s">
         <v>53</v>
       </c>
       <c r="B30" s="32" t="s">
@@ -3001,21 +3223,33 @@
       <c r="C30" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="6"/>
+      <c r="D30" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="60" t="s">
+        <v>235</v>
+      </c>
+      <c r="F30" s="58"/>
+      <c r="G30" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="H30" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="I30" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="J30" s="58"/>
+      <c r="K30" s="32" t="s">
+        <v>212</v>
+      </c>
       <c r="L30" s="32" t="s">
         <v>213</v>
       </c>
       <c r="M30" s="6"/>
     </row>
     <row r="31" spans="1:13" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="39" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="32" t="s">
@@ -3024,21 +3258,33 @@
       <c r="C31" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="6"/>
+      <c r="D31" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="E31" s="60" t="s">
+        <v>239</v>
+      </c>
+      <c r="F31" s="58"/>
+      <c r="G31" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="H31" s="59" t="s">
+        <v>241</v>
+      </c>
+      <c r="I31" s="59" t="s">
+        <v>242</v>
+      </c>
+      <c r="J31" s="58"/>
+      <c r="K31" s="32" t="s">
+        <v>212</v>
+      </c>
       <c r="L31" s="32" t="s">
         <v>213</v>
       </c>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="49" t="s">
+    <row r="32" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="39" t="s">
         <v>166</v>
       </c>
       <c r="B32" s="32" t="s">
@@ -3047,12 +3293,32 @@
       <c r="C32" s="32" t="s">
         <v>189</v>
       </c>
+      <c r="D32" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="E32" s="60" t="s">
+        <v>243</v>
+      </c>
+      <c r="F32" s="58"/>
+      <c r="G32" s="59" t="s">
+        <v>244</v>
+      </c>
+      <c r="H32" s="59" t="s">
+        <v>245</v>
+      </c>
+      <c r="I32" s="59" t="s">
+        <v>246</v>
+      </c>
+      <c r="J32" s="58"/>
+      <c r="K32" s="32" t="s">
+        <v>212</v>
+      </c>
       <c r="L32" s="32" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="49" t="s">
+    <row r="33" spans="1:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="39" t="s">
         <v>167</v>
       </c>
       <c r="B33" s="32" t="s">
@@ -3061,12 +3327,32 @@
       <c r="C33" s="32" t="s">
         <v>190</v>
       </c>
+      <c r="D33" s="56" t="s">
+        <v>214</v>
+      </c>
+      <c r="E33" s="60" t="s">
+        <v>239</v>
+      </c>
+      <c r="F33" s="58"/>
+      <c r="G33" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="H33" s="59" t="s">
+        <v>248</v>
+      </c>
+      <c r="I33" s="59" t="s">
+        <v>249</v>
+      </c>
+      <c r="J33" s="58"/>
+      <c r="K33" s="32" t="s">
+        <v>212</v>
+      </c>
       <c r="L33" s="32" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="49" t="s">
+    <row r="34" spans="1:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="39" t="s">
         <v>168</v>
       </c>
       <c r="B34" s="32" t="s">
@@ -3075,12 +3361,32 @@
       <c r="C34" s="32" t="s">
         <v>191</v>
       </c>
+      <c r="D34" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="60" t="s">
+        <v>220</v>
+      </c>
+      <c r="F34" s="58"/>
+      <c r="G34" s="59" t="s">
+        <v>250</v>
+      </c>
+      <c r="H34" s="59" t="s">
+        <v>251</v>
+      </c>
+      <c r="I34" s="59" t="s">
+        <v>252</v>
+      </c>
+      <c r="J34" s="58"/>
+      <c r="K34" s="32" t="s">
+        <v>212</v>
+      </c>
       <c r="L34" s="32" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="50" t="s">
+      <c r="A35" s="40" t="s">
         <v>169</v>
       </c>
       <c r="B35" s="32" t="s">
@@ -3094,7 +3400,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="40" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="32" t="s">
@@ -3108,7 +3414,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="50" t="s">
+      <c r="A37" s="40" t="s">
         <v>171</v>
       </c>
       <c r="B37" s="32" t="s">
@@ -3122,7 +3428,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="40" t="s">
         <v>172</v>
       </c>
       <c r="B38" s="32" t="s">
@@ -3136,7 +3442,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="50" t="s">
+      <c r="A39" s="40" t="s">
         <v>173</v>
       </c>
       <c r="B39" s="32" t="s">
@@ -3150,7 +3456,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="50" t="s">
+      <c r="A40" s="40" t="s">
         <v>174</v>
       </c>
       <c r="B40" s="32" t="s">
@@ -3164,7 +3470,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="50" t="s">
+      <c r="A41" s="40" t="s">
         <v>175</v>
       </c>
       <c r="B41" s="32" t="s">
@@ -3178,7 +3484,7 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="40" t="s">
         <v>176</v>
       </c>
       <c r="B42" s="32" t="s">
@@ -3192,7 +3498,7 @@
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="50" t="s">
+      <c r="A43" s="40" t="s">
         <v>177</v>
       </c>
       <c r="B43" s="32" t="s">
@@ -3206,7 +3512,7 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="50" t="s">
+      <c r="A44" s="40" t="s">
         <v>178</v>
       </c>
       <c r="B44" s="32" t="s">
@@ -3220,7 +3526,7 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="51" t="s">
+      <c r="A45" s="41" t="s">
         <v>179</v>
       </c>
       <c r="B45" s="32" t="s">
@@ -3234,7 +3540,7 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="51" t="s">
+      <c r="A46" s="41" t="s">
         <v>180</v>
       </c>
       <c r="B46" s="32" t="s">
@@ -3248,7 +3554,7 @@
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="51" t="s">
+      <c r="A47" s="41" t="s">
         <v>181</v>
       </c>
       <c r="B47" s="32" t="s">
@@ -3262,7 +3568,7 @@
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="51" t="s">
+      <c r="A48" s="41" t="s">
         <v>182</v>
       </c>
       <c r="B48" s="32" t="s">
@@ -3276,7 +3582,7 @@
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="51" t="s">
+      <c r="A49" s="41" t="s">
         <v>183</v>
       </c>
       <c r="B49" s="32" t="s">
@@ -3290,7 +3596,7 @@
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="51" t="s">
+      <c r="A50" s="41" t="s">
         <v>184</v>
       </c>
       <c r="B50" s="32" t="s">
@@ -3304,7 +3610,7 @@
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="51" t="s">
+      <c r="A51" s="41" t="s">
         <v>185</v>
       </c>
       <c r="B51" s="32" t="s">
@@ -3315,7 +3621,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="51" t="s">
+      <c r="A52" s="41" t="s">
         <v>186</v>
       </c>
       <c r="B52" s="32" t="s">
@@ -3326,7 +3632,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="51" t="s">
+      <c r="A53" s="41" t="s">
         <v>187</v>
       </c>
       <c r="B53" s="32" t="s">
@@ -3337,7 +3643,7 @@
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="51" t="s">
+      <c r="A54" s="41" t="s">
         <v>188</v>
       </c>
       <c r="B54" s="32" t="s">

</xml_diff>